<commit_message>
Se mejora el javaScript y los formatos Json.
</commit_message>
<xml_diff>
--- a/Complementos.xlsx
+++ b/Complementos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\PycharmProjects\Django_horarios_V6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC70B715-2313-4F1F-9910-988A72E8C95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7CEA0-01B0-44B6-AF97-B9F26B6AD2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E6602D61-97C0-4499-8F33-A12E244B4D86}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -343,8 +343,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{79567F9F-1F4F-4E9D-8582-102D9056CA98}" name="Tabla2" displayName="Tabla2" ref="F2:G57" totalsRowShown="0">
   <autoFilter ref="F2:G57" xr:uid="{79567F9F-1F4F-4E9D-8582-102D9056CA98}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:G44">
-    <sortCondition ref="G2:G44"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F3:G57">
+    <sortCondition ref="G2:G57"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="2" xr3:uid="{9ACF948D-DEC5-4E52-9E94-0DB75641581A}" name="No"/>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517EB25E-5F15-4935-8D9C-647B88A2BAF3}">
   <dimension ref="A2:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +663,7 @@
     <col min="2" max="2" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -762,10 +762,10 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -779,10 +779,10 @@
         <v>14</v>
       </c>
       <c r="F8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -796,18 +796,18 @@
         <v>9</v>
       </c>
       <c r="F9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F10">
-        <v>8</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>68</v>
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -852,322 +852,322 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F16">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s">
-        <v>25</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F17">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F18">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F19">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F20">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G20" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F21">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F22">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
         <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F23">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G23" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F24">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G24" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F25">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G25" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F26">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F27">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G27" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F28">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G28" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F29">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F30">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s">
-        <v>27</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F31">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="G31" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F32">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G32" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F33">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="G33" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F34">
-        <v>32</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="G34" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F35">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="G35" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F36">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G36" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F37">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G37" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F38">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="G38" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F39">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G39" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F40">
-        <v>38</v>
-      </c>
-      <c r="G40" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F41">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="42" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F42">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="G42" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="43" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F43">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="G43" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F44">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G44" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
     </row>
     <row r="45" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F45">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G45" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F46">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G46" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F47">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="G47" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F48">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F49">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G49" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
     </row>
     <row r="50" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F50">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G50" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F51">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="G51" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F52">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="G52" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
     </row>
     <row r="53" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F53">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="G53" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F54">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G54" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F55">
-        <v>53</v>
-      </c>
-      <c r="G55" t="s">
-        <v>67</v>
+        <v>8</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="6:7" x14ac:dyDescent="0.3">
@@ -1180,10 +1180,10 @@
     </row>
     <row r="57" spans="6:7" x14ac:dyDescent="0.3">
       <c r="F57">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G57" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>